<commit_message>
Melhor filtro por pulso encontrado, plot dos parâmetros gerais ainda fazendo
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lesly\Desktop\Lesly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D976C76C-E06F-4962-A89D-D1BD2A49F9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D85DEB3-BD29-4F70-B412-4AE8FAE88C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7716" yWindow="3288" windowWidth="15324" windowHeight="9072" tabRatio="609" activeTab="1" xr2:uid="{764A863F-3A7E-4ACC-8F53-F01996AEDDB5}"/>
+    <workbookView xWindow="11508" yWindow="3504" windowWidth="15324" windowHeight="9072" tabRatio="609" firstSheet="1" activeTab="2" xr2:uid="{764A863F-3A7E-4ACC-8F53-F01996AEDDB5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Resumo %" sheetId="1" r:id="rId1"/>
-    <sheet name="Resumo simplificado" sheetId="2" r:id="rId2"/>
-    <sheet name="Resumo data" sheetId="11" r:id="rId3"/>
+    <sheet name="Resumo por pulso" sheetId="12" r:id="rId1"/>
+    <sheet name="Resumo %" sheetId="1" r:id="rId2"/>
+    <sheet name="Resumo simplificado" sheetId="2" r:id="rId3"/>
+    <sheet name="Resumo data" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3988" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4192" uniqueCount="311">
   <si>
     <t>Pulso</t>
   </si>
@@ -970,9 +971,6 @@
   </si>
   <si>
     <t>38, 26, 66, 25, 24.75</t>
-  </si>
-  <si>
-    <t>ideia das possibilidades ponderadas</t>
   </si>
 </sst>
 </file>
@@ -1357,6 +1355,1021 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B87FEB-9974-4038-87DE-4C74606D219D}">
+  <dimension ref="A1:O27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3">
+        <v>11</v>
+      </c>
+      <c r="L3">
+        <v>62</v>
+      </c>
+      <c r="M3">
+        <v>0.94202020951123899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>9</v>
+      </c>
+      <c r="L4">
+        <v>18</v>
+      </c>
+      <c r="M4">
+        <v>0.97755149231844496</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <v>9</v>
+      </c>
+      <c r="L5">
+        <v>74</v>
+      </c>
+      <c r="M5">
+        <v>0.94894150771882402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>0.96440126611762</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <v>0.96140284098682505</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>22</v>
+      </c>
+      <c r="M8">
+        <v>0.93625335491316797</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9">
+        <v>7</v>
+      </c>
+      <c r="L9">
+        <v>30</v>
+      </c>
+      <c r="M9">
+        <v>0.98505568510328301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <v>14</v>
+      </c>
+      <c r="M10">
+        <v>0.83797236719804202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <v>6</v>
+      </c>
+      <c r="M11">
+        <v>0.96440126611762</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <v>62</v>
+      </c>
+      <c r="M12">
+        <v>0.87122132998973101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13">
+        <v>9</v>
+      </c>
+      <c r="L13">
+        <v>10</v>
+      </c>
+      <c r="M13">
+        <v>0.96140284098682505</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+      <c r="M14">
+        <v>0.96140284098682505</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <v>9</v>
+      </c>
+      <c r="L15">
+        <v>38</v>
+      </c>
+      <c r="M15">
+        <v>0.70219382777156303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16">
+        <v>8</v>
+      </c>
+      <c r="L16">
+        <v>26</v>
+      </c>
+      <c r="M16">
+        <v>0.94937198486445595</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17">
+        <v>9</v>
+      </c>
+      <c r="L17">
+        <v>10</v>
+      </c>
+      <c r="M17">
+        <v>0.96140284098682505</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <v>86</v>
+      </c>
+      <c r="M18">
+        <v>0.89323712907623098</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <v>26</v>
+      </c>
+      <c r="M19">
+        <v>0.94937198486445595</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20">
+        <v>11</v>
+      </c>
+      <c r="L20">
+        <v>74</v>
+      </c>
+      <c r="M20">
+        <v>0.94894150771882402</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21">
+        <v>9</v>
+      </c>
+      <c r="L21">
+        <v>82</v>
+      </c>
+      <c r="M21">
+        <v>0.90218219978078495</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22">
+        <v>10</v>
+      </c>
+      <c r="L22">
+        <v>74</v>
+      </c>
+      <c r="M22">
+        <v>0.94894150771882402</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="L23">
+        <v>90</v>
+      </c>
+      <c r="M23">
+        <v>0.99196465263104205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24">
+        <v>6</v>
+      </c>
+      <c r="L24">
+        <v>10</v>
+      </c>
+      <c r="M24">
+        <v>0.93124316874250501</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K25">
+        <v>7</v>
+      </c>
+      <c r="L25">
+        <v>14</v>
+      </c>
+      <c r="M25">
+        <v>0.965919160916346</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26">
+        <v>4</v>
+      </c>
+      <c r="L26">
+        <v>30</v>
+      </c>
+      <c r="M26">
+        <v>0.88279159320837097</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" t="s">
+        <v>9</v>
+      </c>
+      <c r="K27">
+        <v>9</v>
+      </c>
+      <c r="L27">
+        <v>38</v>
+      </c>
+      <c r="M27">
+        <v>0.92536476108613197</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="M2:N2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4A1C91-8DBE-41E8-9E99-327BF5239A9F}">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -2159,12 +3172,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9C9B8A-0C7C-4AA5-96A3-AC6FE56F36F7}">
-  <dimension ref="A1:O179"/>
+  <dimension ref="A1:O177"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="B180" sqref="B180"/>
+      <selection activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10354,11 +11367,6 @@
         <v>26</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B179" t="s">
-        <v>311</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:B2"/>
@@ -10370,17 +11378,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF244596-3B40-45B3-9455-A9B2C54CE12F}">
   <dimension ref="A1:O352"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="10" max="12" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -23558,6 +24567,7 @@
     <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -23765,18 +24775,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23799,14 +24809,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2782DEE7-7810-4EF6-8898-656A13D527A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B8C3DE9-9DC6-4BB9-B728-23492E9A2F7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -23821,4 +24823,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2782DEE7-7810-4EF6-8898-656A13D527A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>